<commit_message>
Fill out capstone rubric grading form.
</commit_message>
<xml_diff>
--- a/korenak_andrew_cap1/Capstone_1_AndrewKorenak.xlsx
+++ b/korenak_andrew_cap1/Capstone_1_AndrewKorenak.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\tek-korenak-cap1\korenak_andrew_cap1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579A3FBA-E42C-4F01-BE71-EFFBC2BCD0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B947E5C-6808-473E-B1BB-4807A648C357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{05EE201A-0BCA-5646-B296-5AABFBEA194B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="129">
   <si>
     <t>Functionality</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>I had been saving frequently for my app whenever I made changes, but I learned I should have probably done more than 8 commits. I occassionally broke things when I went in and changed a feature, and one time I considered rolling back but my last commit was just too long ago.</t>
+  </si>
+  <si>
+    <t>Team Vikas( solo project)</t>
   </si>
 </sst>
 </file>
@@ -1689,8 +1692,8 @@
   </sheetPr>
   <dimension ref="B2:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1781,8 +1784,8 @@
   </sheetPr>
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1817,6 +1820,16 @@
         <v>4</v>
       </c>
       <c r="B2" s="37"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B3" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="5" spans="1:23" s="10" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
@@ -2611,15 +2624,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FEF7458C51E57141848015B90E19E3FF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12fb0db276e8be4984a0823ffe929ad1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d2a9f884-c2eb-4182-8d97-b2c1069a1e77" xmlns:ns3="ad1dcd44-2c79-421e-996d-e07b6b6a06b7" xmlns:ns4="872877ae-a410-445f-835b-653367d2e530" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f400bb4bb80b6365717ab8834d3c4dc" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="d2a9f884-c2eb-4182-8d97-b2c1069a1e77"/>
@@ -2855,6 +2859,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DCCBC0B-BA77-41C1-B14F-94133CE8E251}">
   <ds:schemaRefs>
@@ -2874,14 +2887,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8A09A7-4930-415E-BC0E-99BBC8E2BDB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01D904D9-6110-4D51-8C80-718FF126E788}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2899,4 +2904,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8A09A7-4930-415E-BC0E-99BBC8E2BDB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>